<commit_message>
Added Test cases for partial circuit cabling in the Test Suite
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/ClassLibrary1/bin/Debug/TestDataFiles/CablingDataSet/2M3U3I.xlsx
+++ b/AutoFirmwareUpgrade/ClassLibrary1/bin/Debug/TestDataFiles/CablingDataSet/2M3U3I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB2D86-2887-4532-A42E-78D6EBEEE1CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D5048C-1DB7-42C8-A08F-466C5FAE697E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Channel</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Channel_Number_DSP2</t>
+  </si>
+  <si>
+    <t>Cabling 3U3I</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G19"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +713,7 @@
         <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
         <v>74</v>

</xml_diff>